<commit_message>
perbaikan menggunakan referensi dibanding vlookup
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanfabella/Documents/kampus merdeka/script/natrya-backup-kampusmerdeka/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65915583-75D2-7C47-97B8-6D4F7DE36F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DA9937-0B53-1247-8CD5-70FB45457137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="500" windowWidth="28040" windowHeight="15620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentee" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="26">
   <si>
     <t>id peserta</t>
   </si>
@@ -237,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -271,9 +271,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -592,7 +589,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,282 +617,582 @@
       <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3">
+        <v>6</v>
+      </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3">
+        <v>9</v>
+      </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3">
+        <v>11</v>
+      </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3">
+        <v>12</v>
+      </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="B14" s="3">
+        <v>13</v>
+      </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="B15" s="3">
+        <v>14</v>
+      </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3">
+        <v>16</v>
+      </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3">
+        <v>17</v>
+      </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="3">
+        <v>18</v>
+      </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="3">
+        <v>19</v>
+      </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3">
+        <v>20</v>
+      </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
+      <c r="B22" s="3">
+        <v>21</v>
+      </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3">
+        <v>23</v>
+      </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
+      <c r="B25" s="3">
+        <v>24</v>
+      </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="B26" s="3">
+        <v>25</v>
+      </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="B27" s="3">
+        <v>26</v>
+      </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="B28" s="3">
+        <v>27</v>
+      </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="B29" s="3">
+        <v>28</v>
+      </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
+      <c r="B30" s="3">
+        <v>29</v>
+      </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
+      <c r="B31" s="3">
+        <v>30</v>
+      </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
@@ -3168,7 +3465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H34" sqref="A34:XFD34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3247,7 +3546,9 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="5"/>
       <c r="E4" s="3"/>
@@ -3272,55 +3573,57 @@
       <c r="L4" s="3">
         <v>0</v>
       </c>
-      <c r="M4" s="14" t="e">
-        <f>VLOOKUP($B4,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N4" s="14" t="e">
-        <f>VLOOKUP($B4,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O4" s="14" t="e">
-        <f>VLOOKUP($B4,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P4" s="14" t="e">
-        <f>VLOOKUP($B4,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M4" s="14" t="str">
+        <f>mentee!G2</f>
+        <v>nim</v>
+      </c>
+      <c r="N4" s="14" t="str">
+        <f>mentee!D2</f>
+        <v>email</v>
+      </c>
+      <c r="O4" s="14" t="str">
+        <f>mentee!E2</f>
+        <v>univ</v>
+      </c>
+      <c r="P4" s="14" t="str">
+        <f>mentee!F2</f>
+        <v>jurusan</v>
       </c>
       <c r="Q4" s="3"/>
-      <c r="R4" s="16" t="str">
+      <c r="R4" s="15" t="str">
         <f>IF(F4&gt;=85,"A",IF(AND(F4&gt;=80,F4&lt;85),"A-",IF(AND(F4&gt;=75,F4&lt;80),"B+",IF(AND(F4&gt;=70,F4&lt;75),"B",IF(AND(F4&gt;=65,F4&lt;70),"B-",IF(AND(F4&gt;=62.5,F4&lt;65),"C+",IF(AND(F4&gt;=60,F4&lt;62.5),"C",IF(AND(F4&gt;=57,F4&lt;60),"C-",IF(AND(F4&gt;=55,F4&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="S4" s="16" t="str">
+      <c r="S4" s="15" t="str">
         <f t="shared" ref="S4:X4" si="0">IF(G4&gt;=85,"A",IF(AND(G4&gt;=80,G4&lt;85),"A-",IF(AND(G4&gt;=75,G4&lt;80),"B+",IF(AND(G4&gt;=70,G4&lt;75),"B",IF(AND(G4&gt;=65,G4&lt;70),"B-",IF(AND(G4&gt;=62.5,G4&lt;65),"C+",IF(AND(G4&gt;=60,G4&lt;62.5),"C",IF(AND(G4&gt;=57,G4&lt;60),"C-",IF(AND(G4&gt;=55,G4&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="T4" s="16" t="str">
+      <c r="T4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
-      <c r="U4" s="16" t="str">
+      <c r="U4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
-      <c r="V4" s="16" t="str">
+      <c r="V4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
-      <c r="W4" s="16" t="str">
+      <c r="W4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
-      <c r="X4" s="16" t="str">
+      <c r="X4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -3345,55 +3648,57 @@
       <c r="L5" s="3">
         <v>0</v>
       </c>
-      <c r="M5" s="14" t="e">
-        <f>VLOOKUP($B5,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N5" s="14" t="e">
-        <f>VLOOKUP($B5,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O5" s="14" t="e">
-        <f>VLOOKUP($B5,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P5" s="14" t="e">
-        <f>VLOOKUP($B5,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M5" s="14" t="str">
+        <f>mentee!G3</f>
+        <v>nim</v>
+      </c>
+      <c r="N5" s="14" t="str">
+        <f>mentee!D3</f>
+        <v>email</v>
+      </c>
+      <c r="O5" s="14" t="str">
+        <f>mentee!E3</f>
+        <v>univ</v>
+      </c>
+      <c r="P5" s="14" t="str">
+        <f>mentee!F3</f>
+        <v>jurusan</v>
       </c>
       <c r="Q5" s="3"/>
-      <c r="R5" s="16" t="str">
+      <c r="R5" s="15" t="str">
         <f t="shared" ref="R5:R30" si="1">IF(F5&gt;=85,"A",IF(AND(F5&gt;=80,F5&lt;85),"A-",IF(AND(F5&gt;=75,F5&lt;80),"B+",IF(AND(F5&gt;=70,F5&lt;75),"B",IF(AND(F5&gt;=65,F5&lt;70),"B-",IF(AND(F5&gt;=62.5,F5&lt;65),"C+",IF(AND(F5&gt;=60,F5&lt;62.5),"C",IF(AND(F5&gt;=57,F5&lt;60),"C-",IF(AND(F5&gt;=55,F5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="S5" s="16" t="str">
+      <c r="S5" s="15" t="str">
         <f t="shared" ref="S5:S30" si="2">IF(G5&gt;=85,"A",IF(AND(G5&gt;=80,G5&lt;85),"A-",IF(AND(G5&gt;=75,G5&lt;80),"B+",IF(AND(G5&gt;=70,G5&lt;75),"B",IF(AND(G5&gt;=65,G5&lt;70),"B-",IF(AND(G5&gt;=62.5,G5&lt;65),"C+",IF(AND(G5&gt;=60,G5&lt;62.5),"C",IF(AND(G5&gt;=57,G5&lt;60),"C-",IF(AND(G5&gt;=55,G5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="T5" s="16" t="str">
+      <c r="T5" s="15" t="str">
         <f t="shared" ref="T5:T30" si="3">IF(H5&gt;=85,"A",IF(AND(H5&gt;=80,H5&lt;85),"A-",IF(AND(H5&gt;=75,H5&lt;80),"B+",IF(AND(H5&gt;=70,H5&lt;75),"B",IF(AND(H5&gt;=65,H5&lt;70),"B-",IF(AND(H5&gt;=62.5,H5&lt;65),"C+",IF(AND(H5&gt;=60,H5&lt;62.5),"C",IF(AND(H5&gt;=57,H5&lt;60),"C-",IF(AND(H5&gt;=55,H5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="U5" s="16" t="str">
+      <c r="U5" s="15" t="str">
         <f t="shared" ref="U5:U30" si="4">IF(I5&gt;=85,"A",IF(AND(I5&gt;=80,I5&lt;85),"A-",IF(AND(I5&gt;=75,I5&lt;80),"B+",IF(AND(I5&gt;=70,I5&lt;75),"B",IF(AND(I5&gt;=65,I5&lt;70),"B-",IF(AND(I5&gt;=62.5,I5&lt;65),"C+",IF(AND(I5&gt;=60,I5&lt;62.5),"C",IF(AND(I5&gt;=57,I5&lt;60),"C-",IF(AND(I5&gt;=55,I5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="V5" s="16" t="str">
+      <c r="V5" s="15" t="str">
         <f t="shared" ref="V5:V30" si="5">IF(J5&gt;=85,"A",IF(AND(J5&gt;=80,J5&lt;85),"A-",IF(AND(J5&gt;=75,J5&lt;80),"B+",IF(AND(J5&gt;=70,J5&lt;75),"B",IF(AND(J5&gt;=65,J5&lt;70),"B-",IF(AND(J5&gt;=62.5,J5&lt;65),"C+",IF(AND(J5&gt;=60,J5&lt;62.5),"C",IF(AND(J5&gt;=57,J5&lt;60),"C-",IF(AND(J5&gt;=55,J5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="W5" s="16" t="str">
+      <c r="W5" s="15" t="str">
         <f t="shared" ref="W5:W30" si="6">IF(K5&gt;=85,"A",IF(AND(K5&gt;=80,K5&lt;85),"A-",IF(AND(K5&gt;=75,K5&lt;80),"B+",IF(AND(K5&gt;=70,K5&lt;75),"B",IF(AND(K5&gt;=65,K5&lt;70),"B-",IF(AND(K5&gt;=62.5,K5&lt;65),"C+",IF(AND(K5&gt;=60,K5&lt;62.5),"C",IF(AND(K5&gt;=57,K5&lt;60),"C-",IF(AND(K5&gt;=55,K5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="X5" s="16" t="str">
+      <c r="X5" s="15" t="str">
         <f t="shared" ref="X5:X30" si="7">IF(L5&gt;=85,"A",IF(AND(L5&gt;=80,L5&lt;85),"A-",IF(AND(L5&gt;=75,L5&lt;80),"B+",IF(AND(L5&gt;=70,L5&lt;75),"B",IF(AND(L5&gt;=65,L5&lt;70),"B-",IF(AND(L5&gt;=62.5,L5&lt;65),"C+",IF(AND(L5&gt;=60,L5&lt;62.5),"C",IF(AND(L5&gt;=57,L5&lt;60),"C-",IF(AND(L5&gt;=55,L5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -3418,55 +3723,57 @@
       <c r="L6" s="3">
         <v>0</v>
       </c>
-      <c r="M6" s="14" t="e">
-        <f>VLOOKUP($B6,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N6" s="14" t="e">
-        <f>VLOOKUP($B6,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O6" s="14" t="e">
-        <f>VLOOKUP($B6,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P6" s="14" t="e">
-        <f>VLOOKUP($B6,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M6" s="14" t="str">
+        <f>mentee!G4</f>
+        <v>nim</v>
+      </c>
+      <c r="N6" s="14" t="str">
+        <f>mentee!D4</f>
+        <v>email</v>
+      </c>
+      <c r="O6" s="14" t="str">
+        <f>mentee!E4</f>
+        <v>univ</v>
+      </c>
+      <c r="P6" s="14" t="str">
+        <f>mentee!F4</f>
+        <v>jurusan</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="16" t="str">
+      <c r="R6" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S6" s="16" t="str">
+      <c r="S6" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T6" s="16" t="str">
+      <c r="T6" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U6" s="16" t="str">
+      <c r="U6" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V6" s="16" t="str">
+      <c r="V6" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W6" s="16" t="str">
+      <c r="W6" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X6" s="16" t="str">
+      <c r="X6" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -3491,55 +3798,57 @@
       <c r="L7" s="3">
         <v>0</v>
       </c>
-      <c r="M7" s="14" t="e">
-        <f>VLOOKUP($B7,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N7" s="14" t="e">
-        <f>VLOOKUP($B7,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O7" s="14" t="e">
-        <f>VLOOKUP($B7,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P7" s="14" t="e">
-        <f>VLOOKUP($B7,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M7" s="14" t="str">
+        <f>mentee!G5</f>
+        <v>nim</v>
+      </c>
+      <c r="N7" s="14" t="str">
+        <f>mentee!D5</f>
+        <v>email</v>
+      </c>
+      <c r="O7" s="14" t="str">
+        <f>mentee!E5</f>
+        <v>univ</v>
+      </c>
+      <c r="P7" s="14" t="str">
+        <f>mentee!F5</f>
+        <v>jurusan</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="16" t="str">
+      <c r="R7" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S7" s="16" t="str">
+      <c r="S7" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T7" s="16" t="str">
+      <c r="T7" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U7" s="16" t="str">
+      <c r="U7" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V7" s="16" t="str">
+      <c r="V7" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W7" s="16" t="str">
+      <c r="W7" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X7" s="16" t="str">
+      <c r="X7" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -3564,55 +3873,57 @@
       <c r="L8" s="3">
         <v>0</v>
       </c>
-      <c r="M8" s="14" t="e">
-        <f>VLOOKUP($B8,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N8" s="14" t="e">
-        <f>VLOOKUP($B8,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O8" s="14" t="e">
-        <f>VLOOKUP($B8,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P8" s="14" t="e">
-        <f>VLOOKUP($B8,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M8" s="14" t="str">
+        <f>mentee!G6</f>
+        <v>nim</v>
+      </c>
+      <c r="N8" s="14" t="str">
+        <f>mentee!D6</f>
+        <v>email</v>
+      </c>
+      <c r="O8" s="14" t="str">
+        <f>mentee!E6</f>
+        <v>univ</v>
+      </c>
+      <c r="P8" s="14" t="str">
+        <f>mentee!F6</f>
+        <v>jurusan</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="16" t="str">
+      <c r="R8" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S8" s="16" t="str">
+      <c r="S8" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T8" s="16" t="str">
+      <c r="T8" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U8" s="16" t="str">
+      <c r="U8" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V8" s="16" t="str">
+      <c r="V8" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W8" s="16" t="str">
+      <c r="W8" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X8" s="16" t="str">
+      <c r="X8" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -3637,55 +3948,57 @@
       <c r="L9" s="3">
         <v>0</v>
       </c>
-      <c r="M9" s="14" t="e">
-        <f>VLOOKUP($B9,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N9" s="14" t="e">
-        <f>VLOOKUP($B9,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O9" s="14" t="e">
-        <f>VLOOKUP($B9,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P9" s="14" t="e">
-        <f>VLOOKUP($B9,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M9" s="14" t="str">
+        <f>mentee!G7</f>
+        <v>nim</v>
+      </c>
+      <c r="N9" s="14" t="str">
+        <f>mentee!D7</f>
+        <v>email</v>
+      </c>
+      <c r="O9" s="14" t="str">
+        <f>mentee!E7</f>
+        <v>univ</v>
+      </c>
+      <c r="P9" s="14" t="str">
+        <f>mentee!F7</f>
+        <v>jurusan</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="16" t="str">
+      <c r="R9" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S9" s="16" t="str">
+      <c r="S9" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T9" s="16" t="str">
+      <c r="T9" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U9" s="16" t="str">
+      <c r="U9" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V9" s="16" t="str">
+      <c r="V9" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W9" s="16" t="str">
+      <c r="W9" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X9" s="16" t="str">
+      <c r="X9" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3">
+        <v>7</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -3710,55 +4023,57 @@
       <c r="L10" s="3">
         <v>0</v>
       </c>
-      <c r="M10" s="14" t="e">
-        <f>VLOOKUP($B10,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N10" s="14" t="e">
-        <f>VLOOKUP($B10,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O10" s="14" t="e">
-        <f>VLOOKUP($B10,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P10" s="14" t="e">
-        <f>VLOOKUP($B10,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M10" s="14" t="str">
+        <f>mentee!G8</f>
+        <v>nim</v>
+      </c>
+      <c r="N10" s="14" t="str">
+        <f>mentee!D8</f>
+        <v>email</v>
+      </c>
+      <c r="O10" s="14" t="str">
+        <f>mentee!E8</f>
+        <v>univ</v>
+      </c>
+      <c r="P10" s="14" t="str">
+        <f>mentee!F8</f>
+        <v>jurusan</v>
       </c>
       <c r="Q10" s="3"/>
-      <c r="R10" s="16" t="str">
+      <c r="R10" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S10" s="16" t="str">
+      <c r="S10" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T10" s="16" t="str">
+      <c r="T10" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U10" s="16" t="str">
+      <c r="U10" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V10" s="16" t="str">
+      <c r="V10" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W10" s="16" t="str">
+      <c r="W10" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X10" s="16" t="str">
+      <c r="X10" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <v>8</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -3783,55 +4098,57 @@
       <c r="L11" s="3">
         <v>0</v>
       </c>
-      <c r="M11" s="14" t="e">
-        <f>VLOOKUP($B11,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N11" s="14" t="e">
-        <f>VLOOKUP($B11,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O11" s="14" t="e">
-        <f>VLOOKUP($B11,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P11" s="14" t="e">
-        <f>VLOOKUP($B11,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M11" s="14" t="str">
+        <f>mentee!G9</f>
+        <v>nim</v>
+      </c>
+      <c r="N11" s="14" t="str">
+        <f>mentee!D9</f>
+        <v>email</v>
+      </c>
+      <c r="O11" s="14" t="str">
+        <f>mentee!E9</f>
+        <v>univ</v>
+      </c>
+      <c r="P11" s="14" t="str">
+        <f>mentee!F9</f>
+        <v>jurusan</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="16" t="str">
+      <c r="R11" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S11" s="16" t="str">
+      <c r="S11" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T11" s="16" t="str">
+      <c r="T11" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U11" s="16" t="str">
+      <c r="U11" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V11" s="16" t="str">
+      <c r="V11" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W11" s="16" t="str">
+      <c r="W11" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X11" s="16" t="str">
+      <c r="X11" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3">
+        <v>9</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -3856,55 +4173,57 @@
       <c r="L12" s="3">
         <v>0</v>
       </c>
-      <c r="M12" s="14" t="e">
-        <f>VLOOKUP($B12,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N12" s="14" t="e">
-        <f>VLOOKUP($B12,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O12" s="14" t="e">
-        <f>VLOOKUP($B12,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P12" s="14" t="e">
-        <f>VLOOKUP($B12,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M12" s="14" t="str">
+        <f>mentee!G10</f>
+        <v>nim</v>
+      </c>
+      <c r="N12" s="14" t="str">
+        <f>mentee!D10</f>
+        <v>email</v>
+      </c>
+      <c r="O12" s="14" t="str">
+        <f>mentee!E10</f>
+        <v>univ</v>
+      </c>
+      <c r="P12" s="14" t="str">
+        <f>mentee!F10</f>
+        <v>jurusan</v>
       </c>
       <c r="Q12" s="3"/>
-      <c r="R12" s="16" t="str">
+      <c r="R12" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S12" s="16" t="str">
+      <c r="S12" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T12" s="16" t="str">
+      <c r="T12" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U12" s="16" t="str">
+      <c r="U12" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V12" s="16" t="str">
+      <c r="V12" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W12" s="16" t="str">
+      <c r="W12" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X12" s="16" t="str">
+      <c r="X12" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3">
+        <v>10</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -3929,55 +4248,57 @@
       <c r="L13" s="3">
         <v>0</v>
       </c>
-      <c r="M13" s="14" t="e">
-        <f>VLOOKUP($B13,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N13" s="14" t="e">
-        <f>VLOOKUP($B13,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O13" s="14" t="e">
-        <f>VLOOKUP($B13,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P13" s="14" t="e">
-        <f>VLOOKUP($B13,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M13" s="14" t="str">
+        <f>mentee!G11</f>
+        <v>nim</v>
+      </c>
+      <c r="N13" s="14" t="str">
+        <f>mentee!D11</f>
+        <v>email</v>
+      </c>
+      <c r="O13" s="14" t="str">
+        <f>mentee!E11</f>
+        <v>univ</v>
+      </c>
+      <c r="P13" s="14" t="str">
+        <f>mentee!F11</f>
+        <v>jurusan</v>
       </c>
       <c r="Q13" s="3"/>
-      <c r="R13" s="16" t="str">
+      <c r="R13" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S13" s="16" t="str">
+      <c r="S13" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T13" s="16" t="str">
+      <c r="T13" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U13" s="16" t="str">
+      <c r="U13" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V13" s="16" t="str">
+      <c r="V13" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W13" s="16" t="str">
+      <c r="W13" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X13" s="16" t="str">
+      <c r="X13" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="B14" s="3">
+        <v>11</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -4002,55 +4323,57 @@
       <c r="L14" s="3">
         <v>0</v>
       </c>
-      <c r="M14" s="14" t="e">
-        <f>VLOOKUP($B14,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N14" s="14" t="e">
-        <f>VLOOKUP($B14,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O14" s="14" t="e">
-        <f>VLOOKUP($B14,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P14" s="14" t="e">
-        <f>VLOOKUP($B14,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M14" s="14" t="str">
+        <f>mentee!G12</f>
+        <v>nim</v>
+      </c>
+      <c r="N14" s="14" t="str">
+        <f>mentee!D12</f>
+        <v>email</v>
+      </c>
+      <c r="O14" s="14" t="str">
+        <f>mentee!E12</f>
+        <v>univ</v>
+      </c>
+      <c r="P14" s="14" t="str">
+        <f>mentee!F12</f>
+        <v>jurusan</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="16" t="str">
+      <c r="R14" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S14" s="16" t="str">
+      <c r="S14" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T14" s="16" t="str">
+      <c r="T14" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U14" s="16" t="str">
+      <c r="U14" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V14" s="16" t="str">
+      <c r="V14" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W14" s="16" t="str">
+      <c r="W14" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X14" s="16" t="str">
+      <c r="X14" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="B15" s="3">
+        <v>12</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -4075,55 +4398,57 @@
       <c r="L15" s="3">
         <v>0</v>
       </c>
-      <c r="M15" s="14" t="e">
-        <f>VLOOKUP($B15,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N15" s="14" t="e">
-        <f>VLOOKUP($B15,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O15" s="14" t="e">
-        <f>VLOOKUP($B15,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P15" s="14" t="e">
-        <f>VLOOKUP($B15,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M15" s="14" t="str">
+        <f>mentee!G13</f>
+        <v>nim</v>
+      </c>
+      <c r="N15" s="14" t="str">
+        <f>mentee!D13</f>
+        <v>email</v>
+      </c>
+      <c r="O15" s="14" t="str">
+        <f>mentee!E13</f>
+        <v>univ</v>
+      </c>
+      <c r="P15" s="14" t="str">
+        <f>mentee!F13</f>
+        <v>jurusan</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="16" t="str">
+      <c r="R15" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S15" s="16" t="str">
+      <c r="S15" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T15" s="16" t="str">
+      <c r="T15" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U15" s="16" t="str">
+      <c r="U15" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V15" s="16" t="str">
+      <c r="V15" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W15" s="16" t="str">
+      <c r="W15" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X15" s="16" t="str">
+      <c r="X15" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="3">
+        <v>13</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -4148,55 +4473,57 @@
       <c r="L16" s="3">
         <v>0</v>
       </c>
-      <c r="M16" s="14" t="e">
-        <f>VLOOKUP($B16,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N16" s="14" t="e">
-        <f>VLOOKUP($B16,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O16" s="14" t="e">
-        <f>VLOOKUP($B16,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P16" s="14" t="e">
-        <f>VLOOKUP($B16,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M16" s="14" t="str">
+        <f>mentee!G14</f>
+        <v>nim</v>
+      </c>
+      <c r="N16" s="14" t="str">
+        <f>mentee!D14</f>
+        <v>email</v>
+      </c>
+      <c r="O16" s="14" t="str">
+        <f>mentee!E14</f>
+        <v>univ</v>
+      </c>
+      <c r="P16" s="14" t="str">
+        <f>mentee!F14</f>
+        <v>jurusan</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="16" t="str">
+      <c r="R16" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S16" s="16" t="str">
+      <c r="S16" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T16" s="16" t="str">
+      <c r="T16" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U16" s="16" t="str">
+      <c r="U16" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V16" s="16" t="str">
+      <c r="V16" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W16" s="16" t="str">
+      <c r="W16" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X16" s="16" t="str">
+      <c r="X16" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3">
+        <v>14</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -4221,55 +4548,57 @@
       <c r="L17" s="3">
         <v>0</v>
       </c>
-      <c r="M17" s="14" t="e">
-        <f>VLOOKUP($B17,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N17" s="14" t="e">
-        <f>VLOOKUP($B17,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O17" s="14" t="e">
-        <f>VLOOKUP($B17,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P17" s="14" t="e">
-        <f>VLOOKUP($B17,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M17" s="14" t="str">
+        <f>mentee!G15</f>
+        <v>nim</v>
+      </c>
+      <c r="N17" s="14" t="str">
+        <f>mentee!D15</f>
+        <v>email</v>
+      </c>
+      <c r="O17" s="14" t="str">
+        <f>mentee!E15</f>
+        <v>univ</v>
+      </c>
+      <c r="P17" s="14" t="str">
+        <f>mentee!F15</f>
+        <v>jurusan</v>
       </c>
       <c r="Q17" s="3"/>
-      <c r="R17" s="16" t="str">
+      <c r="R17" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S17" s="16" t="str">
+      <c r="S17" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T17" s="16" t="str">
+      <c r="T17" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U17" s="16" t="str">
+      <c r="U17" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V17" s="16" t="str">
+      <c r="V17" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W17" s="16" t="str">
+      <c r="W17" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X17" s="16" t="str">
+      <c r="X17" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3">
+        <v>15</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -4294,55 +4623,57 @@
       <c r="L18" s="3">
         <v>0</v>
       </c>
-      <c r="M18" s="14" t="e">
-        <f>VLOOKUP($B18,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N18" s="14" t="e">
-        <f>VLOOKUP($B18,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O18" s="14" t="e">
-        <f>VLOOKUP($B18,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P18" s="14" t="e">
-        <f>VLOOKUP($B18,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M18" s="14" t="str">
+        <f>mentee!G16</f>
+        <v>nim</v>
+      </c>
+      <c r="N18" s="14" t="str">
+        <f>mentee!D16</f>
+        <v>email</v>
+      </c>
+      <c r="O18" s="14" t="str">
+        <f>mentee!E16</f>
+        <v>univ</v>
+      </c>
+      <c r="P18" s="14" t="str">
+        <f>mentee!F16</f>
+        <v>jurusan</v>
       </c>
       <c r="Q18" s="3"/>
-      <c r="R18" s="16" t="str">
+      <c r="R18" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S18" s="16" t="str">
+      <c r="S18" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T18" s="16" t="str">
+      <c r="T18" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U18" s="16" t="str">
+      <c r="U18" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V18" s="16" t="str">
+      <c r="V18" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W18" s="16" t="str">
+      <c r="W18" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X18" s="16" t="str">
+      <c r="X18" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="3">
+        <v>16</v>
+      </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -4367,55 +4698,57 @@
       <c r="L19" s="3">
         <v>0</v>
       </c>
-      <c r="M19" s="14" t="e">
-        <f>VLOOKUP($B19,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N19" s="14" t="e">
-        <f>VLOOKUP($B19,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O19" s="14" t="e">
-        <f>VLOOKUP($B19,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P19" s="14" t="e">
-        <f>VLOOKUP($B19,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M19" s="14" t="str">
+        <f>mentee!G17</f>
+        <v>nim</v>
+      </c>
+      <c r="N19" s="14" t="str">
+        <f>mentee!D17</f>
+        <v>email</v>
+      </c>
+      <c r="O19" s="14" t="str">
+        <f>mentee!E17</f>
+        <v>univ</v>
+      </c>
+      <c r="P19" s="14" t="str">
+        <f>mentee!F17</f>
+        <v>jurusan</v>
       </c>
       <c r="Q19" s="3"/>
-      <c r="R19" s="16" t="str">
+      <c r="R19" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S19" s="16" t="str">
+      <c r="S19" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T19" s="16" t="str">
+      <c r="T19" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U19" s="16" t="str">
+      <c r="U19" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V19" s="16" t="str">
+      <c r="V19" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W19" s="16" t="str">
+      <c r="W19" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X19" s="16" t="str">
+      <c r="X19" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="3">
+        <v>17</v>
+      </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -4440,55 +4773,57 @@
       <c r="L20" s="3">
         <v>0</v>
       </c>
-      <c r="M20" s="14" t="e">
-        <f>VLOOKUP($B20,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N20" s="14" t="e">
-        <f>VLOOKUP($B20,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O20" s="14" t="e">
-        <f>VLOOKUP($B20,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P20" s="14" t="e">
-        <f>VLOOKUP($B20,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M20" s="14" t="str">
+        <f>mentee!G18</f>
+        <v>nim</v>
+      </c>
+      <c r="N20" s="14" t="str">
+        <f>mentee!D18</f>
+        <v>email</v>
+      </c>
+      <c r="O20" s="14" t="str">
+        <f>mentee!E18</f>
+        <v>univ</v>
+      </c>
+      <c r="P20" s="14" t="str">
+        <f>mentee!F18</f>
+        <v>jurusan</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="16" t="str">
+      <c r="R20" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S20" s="16" t="str">
+      <c r="S20" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T20" s="16" t="str">
+      <c r="T20" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U20" s="16" t="str">
+      <c r="U20" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V20" s="16" t="str">
+      <c r="V20" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W20" s="16" t="str">
+      <c r="W20" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X20" s="16" t="str">
+      <c r="X20" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3">
+        <v>18</v>
+      </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -4513,55 +4848,57 @@
       <c r="L21" s="3">
         <v>0</v>
       </c>
-      <c r="M21" s="14" t="e">
-        <f>VLOOKUP($B21,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N21" s="14" t="e">
-        <f>VLOOKUP($B21,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O21" s="14" t="e">
-        <f>VLOOKUP($B21,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P21" s="14" t="e">
-        <f>VLOOKUP($B21,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M21" s="14" t="str">
+        <f>mentee!G19</f>
+        <v>nim</v>
+      </c>
+      <c r="N21" s="14" t="str">
+        <f>mentee!D19</f>
+        <v>email</v>
+      </c>
+      <c r="O21" s="14" t="str">
+        <f>mentee!E19</f>
+        <v>univ</v>
+      </c>
+      <c r="P21" s="14" t="str">
+        <f>mentee!F19</f>
+        <v>jurusan</v>
       </c>
       <c r="Q21" s="3"/>
-      <c r="R21" s="16" t="str">
+      <c r="R21" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S21" s="16" t="str">
+      <c r="S21" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T21" s="16" t="str">
+      <c r="T21" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U21" s="16" t="str">
+      <c r="U21" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V21" s="16" t="str">
+      <c r="V21" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W21" s="16" t="str">
+      <c r="W21" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X21" s="16" t="str">
+      <c r="X21" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
+      <c r="B22" s="3">
+        <v>19</v>
+      </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -4586,55 +4923,57 @@
       <c r="L22" s="3">
         <v>0</v>
       </c>
-      <c r="M22" s="14" t="e">
-        <f>VLOOKUP($B22,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N22" s="14" t="e">
-        <f>VLOOKUP($B22,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O22" s="14" t="e">
-        <f>VLOOKUP($B22,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P22" s="14" t="e">
-        <f>VLOOKUP($B22,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M22" s="14" t="str">
+        <f>mentee!G20</f>
+        <v>nim</v>
+      </c>
+      <c r="N22" s="14" t="str">
+        <f>mentee!D20</f>
+        <v>email</v>
+      </c>
+      <c r="O22" s="14" t="str">
+        <f>mentee!E20</f>
+        <v>univ</v>
+      </c>
+      <c r="P22" s="14" t="str">
+        <f>mentee!F20</f>
+        <v>jurusan</v>
       </c>
       <c r="Q22" s="3"/>
-      <c r="R22" s="16" t="str">
+      <c r="R22" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S22" s="16" t="str">
+      <c r="S22" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T22" s="16" t="str">
+      <c r="T22" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U22" s="16" t="str">
+      <c r="U22" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V22" s="16" t="str">
+      <c r="V22" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W22" s="16" t="str">
+      <c r="W22" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X22" s="16" t="str">
+      <c r="X22" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3">
+        <v>20</v>
+      </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -4659,55 +4998,57 @@
       <c r="L23" s="3">
         <v>0</v>
       </c>
-      <c r="M23" s="14" t="e">
-        <f>VLOOKUP($B23,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N23" s="14" t="e">
-        <f>VLOOKUP($B23,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O23" s="14" t="e">
-        <f>VLOOKUP($B23,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P23" s="14" t="e">
-        <f>VLOOKUP($B23,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M23" s="14" t="str">
+        <f>mentee!G21</f>
+        <v>nim</v>
+      </c>
+      <c r="N23" s="14" t="str">
+        <f>mentee!D21</f>
+        <v>email</v>
+      </c>
+      <c r="O23" s="14" t="str">
+        <f>mentee!E21</f>
+        <v>univ</v>
+      </c>
+      <c r="P23" s="14" t="str">
+        <f>mentee!F21</f>
+        <v>jurusan</v>
       </c>
       <c r="Q23" s="3"/>
-      <c r="R23" s="16" t="str">
+      <c r="R23" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S23" s="16" t="str">
+      <c r="S23" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T23" s="16" t="str">
+      <c r="T23" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U23" s="16" t="str">
+      <c r="U23" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V23" s="16" t="str">
+      <c r="V23" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W23" s="16" t="str">
+      <c r="W23" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X23" s="16" t="str">
+      <c r="X23" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3">
+        <v>21</v>
+      </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -4732,55 +5073,57 @@
       <c r="L24" s="3">
         <v>0</v>
       </c>
-      <c r="M24" s="14" t="e">
-        <f>VLOOKUP($B24,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N24" s="14" t="e">
-        <f>VLOOKUP($B24,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O24" s="14" t="e">
-        <f>VLOOKUP($B24,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P24" s="14" t="e">
-        <f>VLOOKUP($B24,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M24" s="14" t="str">
+        <f>mentee!G22</f>
+        <v>nim</v>
+      </c>
+      <c r="N24" s="14" t="str">
+        <f>mentee!D22</f>
+        <v>email</v>
+      </c>
+      <c r="O24" s="14" t="str">
+        <f>mentee!E22</f>
+        <v>univ</v>
+      </c>
+      <c r="P24" s="14" t="str">
+        <f>mentee!F22</f>
+        <v>jurusan</v>
       </c>
       <c r="Q24" s="3"/>
-      <c r="R24" s="16" t="str">
+      <c r="R24" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S24" s="16" t="str">
+      <c r="S24" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T24" s="16" t="str">
+      <c r="T24" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U24" s="16" t="str">
+      <c r="U24" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V24" s="16" t="str">
+      <c r="V24" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W24" s="16" t="str">
+      <c r="W24" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X24" s="16" t="str">
+      <c r="X24" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
+      <c r="B25" s="3">
+        <v>22</v>
+      </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -4805,55 +5148,57 @@
       <c r="L25" s="3">
         <v>0</v>
       </c>
-      <c r="M25" s="14" t="e">
-        <f>VLOOKUP($B25,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N25" s="14" t="e">
-        <f>VLOOKUP($B25,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O25" s="14" t="e">
-        <f>VLOOKUP($B25,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P25" s="14" t="e">
-        <f>VLOOKUP($B25,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M25" s="14" t="str">
+        <f>mentee!G23</f>
+        <v>nim</v>
+      </c>
+      <c r="N25" s="14" t="str">
+        <f>mentee!D23</f>
+        <v>email</v>
+      </c>
+      <c r="O25" s="14" t="str">
+        <f>mentee!E23</f>
+        <v>univ</v>
+      </c>
+      <c r="P25" s="14" t="str">
+        <f>mentee!F23</f>
+        <v>jurusan</v>
       </c>
       <c r="Q25" s="3"/>
-      <c r="R25" s="16" t="str">
+      <c r="R25" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S25" s="16" t="str">
+      <c r="S25" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T25" s="16" t="str">
+      <c r="T25" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U25" s="16" t="str">
+      <c r="U25" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V25" s="16" t="str">
+      <c r="V25" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W25" s="16" t="str">
+      <c r="W25" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X25" s="16" t="str">
+      <c r="X25" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="B26" s="3">
+        <v>23</v>
+      </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -4878,55 +5223,57 @@
       <c r="L26" s="3">
         <v>0</v>
       </c>
-      <c r="M26" s="14" t="e">
-        <f>VLOOKUP($B26,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N26" s="14" t="e">
-        <f>VLOOKUP($B26,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O26" s="14" t="e">
-        <f>VLOOKUP($B26,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P26" s="14" t="e">
-        <f>VLOOKUP($B26,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M26" s="14" t="str">
+        <f>mentee!G24</f>
+        <v>nim</v>
+      </c>
+      <c r="N26" s="14" t="str">
+        <f>mentee!D24</f>
+        <v>email</v>
+      </c>
+      <c r="O26" s="14" t="str">
+        <f>mentee!E24</f>
+        <v>univ</v>
+      </c>
+      <c r="P26" s="14" t="str">
+        <f>mentee!F24</f>
+        <v>jurusan</v>
       </c>
       <c r="Q26" s="3"/>
-      <c r="R26" s="16" t="str">
+      <c r="R26" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S26" s="16" t="str">
+      <c r="S26" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T26" s="16" t="str">
+      <c r="T26" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U26" s="16" t="str">
+      <c r="U26" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V26" s="16" t="str">
+      <c r="V26" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W26" s="16" t="str">
+      <c r="W26" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X26" s="16" t="str">
+      <c r="X26" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="B27" s="3">
+        <v>24</v>
+      </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -4951,55 +5298,57 @@
       <c r="L27" s="3">
         <v>0</v>
       </c>
-      <c r="M27" s="14" t="e">
-        <f>VLOOKUP($B27,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N27" s="14" t="e">
-        <f>VLOOKUP($B27,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O27" s="14" t="e">
-        <f>VLOOKUP($B27,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P27" s="14" t="e">
-        <f>VLOOKUP($B27,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M27" s="14" t="str">
+        <f>mentee!G25</f>
+        <v>nim</v>
+      </c>
+      <c r="N27" s="14" t="str">
+        <f>mentee!D25</f>
+        <v>email</v>
+      </c>
+      <c r="O27" s="14" t="str">
+        <f>mentee!E25</f>
+        <v>univ</v>
+      </c>
+      <c r="P27" s="14" t="str">
+        <f>mentee!F25</f>
+        <v>jurusan</v>
       </c>
       <c r="Q27" s="3"/>
-      <c r="R27" s="16" t="str">
+      <c r="R27" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S27" s="16" t="str">
+      <c r="S27" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T27" s="16" t="str">
+      <c r="T27" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U27" s="16" t="str">
+      <c r="U27" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V27" s="16" t="str">
+      <c r="V27" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W27" s="16" t="str">
+      <c r="W27" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X27" s="16" t="str">
+      <c r="X27" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="B28" s="3">
+        <v>25</v>
+      </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -5024,55 +5373,57 @@
       <c r="L28" s="3">
         <v>0</v>
       </c>
-      <c r="M28" s="14" t="e">
-        <f>VLOOKUP($B28,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N28" s="14" t="e">
-        <f>VLOOKUP($B28,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O28" s="14" t="e">
-        <f>VLOOKUP($B28,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P28" s="14" t="e">
-        <f>VLOOKUP($B28,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M28" s="14" t="str">
+        <f>mentee!G26</f>
+        <v>nim</v>
+      </c>
+      <c r="N28" s="14" t="str">
+        <f>mentee!D26</f>
+        <v>email</v>
+      </c>
+      <c r="O28" s="14" t="str">
+        <f>mentee!E26</f>
+        <v>univ</v>
+      </c>
+      <c r="P28" s="14" t="str">
+        <f>mentee!F26</f>
+        <v>jurusan</v>
       </c>
       <c r="Q28" s="3"/>
-      <c r="R28" s="16" t="str">
+      <c r="R28" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S28" s="16" t="str">
+      <c r="S28" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T28" s="16" t="str">
+      <c r="T28" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U28" s="16" t="str">
+      <c r="U28" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V28" s="16" t="str">
+      <c r="V28" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W28" s="16" t="str">
+      <c r="W28" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X28" s="16" t="str">
+      <c r="X28" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="B29" s="3">
+        <v>26</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -5097,55 +5448,57 @@
       <c r="L29" s="3">
         <v>0</v>
       </c>
-      <c r="M29" s="14" t="e">
-        <f>VLOOKUP($B29,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N29" s="14" t="e">
-        <f>VLOOKUP($B29,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O29" s="14" t="e">
-        <f>VLOOKUP($B29,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P29" s="14" t="e">
-        <f>VLOOKUP($B29,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M29" s="14" t="str">
+        <f>mentee!G27</f>
+        <v>nim</v>
+      </c>
+      <c r="N29" s="14" t="str">
+        <f>mentee!D27</f>
+        <v>email</v>
+      </c>
+      <c r="O29" s="14" t="str">
+        <f>mentee!E27</f>
+        <v>univ</v>
+      </c>
+      <c r="P29" s="14" t="str">
+        <f>mentee!F27</f>
+        <v>jurusan</v>
       </c>
       <c r="Q29" s="3"/>
-      <c r="R29" s="16" t="str">
+      <c r="R29" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S29" s="16" t="str">
+      <c r="S29" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T29" s="16" t="str">
+      <c r="T29" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U29" s="16" t="str">
+      <c r="U29" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V29" s="16" t="str">
+      <c r="V29" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W29" s="16" t="str">
+      <c r="W29" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X29" s="16" t="str">
+      <c r="X29" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
+      <c r="B30" s="3">
+        <v>27</v>
+      </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -5170,55 +5523,57 @@
       <c r="L30" s="3">
         <v>0</v>
       </c>
-      <c r="M30" s="14" t="e">
-        <f>VLOOKUP($B30,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N30" s="14" t="e">
-        <f>VLOOKUP($B30,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O30" s="14" t="e">
-        <f>VLOOKUP($B30,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P30" s="14" t="e">
-        <f>VLOOKUP($B30,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M30" s="14" t="str">
+        <f>mentee!G28</f>
+        <v>nim</v>
+      </c>
+      <c r="N30" s="14" t="str">
+        <f>mentee!D28</f>
+        <v>email</v>
+      </c>
+      <c r="O30" s="14" t="str">
+        <f>mentee!E28</f>
+        <v>univ</v>
+      </c>
+      <c r="P30" s="14" t="str">
+        <f>mentee!F28</f>
+        <v>jurusan</v>
       </c>
       <c r="Q30" s="3"/>
-      <c r="R30" s="16" t="str">
+      <c r="R30" s="15" t="str">
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="S30" s="16" t="str">
+      <c r="S30" s="15" t="str">
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="T30" s="16" t="str">
+      <c r="T30" s="15" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
       </c>
-      <c r="U30" s="16" t="str">
+      <c r="U30" s="15" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
       </c>
-      <c r="V30" s="16" t="str">
+      <c r="V30" s="15" t="str">
         <f t="shared" si="5"/>
         <v>E</v>
       </c>
-      <c r="W30" s="16" t="str">
+      <c r="W30" s="15" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
       </c>
-      <c r="X30" s="16" t="str">
+      <c r="X30" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
+      <c r="B31" s="3">
+        <v>28</v>
+      </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -5243,55 +5598,57 @@
       <c r="L31" s="3">
         <v>0</v>
       </c>
-      <c r="M31" s="14" t="e">
-        <f>VLOOKUP($B31,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N31" s="14" t="e">
-        <f>VLOOKUP($B31,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O31" s="14" t="e">
-        <f>VLOOKUP($B31,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P31" s="14" t="e">
-        <f>VLOOKUP($B31,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M31" s="14" t="str">
+        <f>mentee!G29</f>
+        <v>nim</v>
+      </c>
+      <c r="N31" s="14" t="str">
+        <f>mentee!D29</f>
+        <v>email</v>
+      </c>
+      <c r="O31" s="14" t="str">
+        <f>mentee!E29</f>
+        <v>univ</v>
+      </c>
+      <c r="P31" s="14" t="str">
+        <f>mentee!F29</f>
+        <v>jurusan</v>
       </c>
       <c r="Q31" s="3"/>
-      <c r="R31" s="16" t="str">
+      <c r="R31" s="15" t="str">
         <f t="shared" ref="R31:R34" si="8">IF(F31&gt;=85,"A",IF(AND(F31&gt;=80,F31&lt;85),"A-",IF(AND(F31&gt;=75,F31&lt;80),"B+",IF(AND(F31&gt;=70,F31&lt;75),"B",IF(AND(F31&gt;=65,F31&lt;70),"B-",IF(AND(F31&gt;=62.5,F31&lt;65),"C+",IF(AND(F31&gt;=60,F31&lt;62.5),"C",IF(AND(F31&gt;=57,F31&lt;60),"C-",IF(AND(F31&gt;=55,F31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="S31" s="16" t="str">
+      <c r="S31" s="15" t="str">
         <f t="shared" ref="S31:S34" si="9">IF(G31&gt;=85,"A",IF(AND(G31&gt;=80,G31&lt;85),"A-",IF(AND(G31&gt;=75,G31&lt;80),"B+",IF(AND(G31&gt;=70,G31&lt;75),"B",IF(AND(G31&gt;=65,G31&lt;70),"B-",IF(AND(G31&gt;=62.5,G31&lt;65),"C+",IF(AND(G31&gt;=60,G31&lt;62.5),"C",IF(AND(G31&gt;=57,G31&lt;60),"C-",IF(AND(G31&gt;=55,G31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="T31" s="16" t="str">
+      <c r="T31" s="15" t="str">
         <f t="shared" ref="T31:T34" si="10">IF(H31&gt;=85,"A",IF(AND(H31&gt;=80,H31&lt;85),"A-",IF(AND(H31&gt;=75,H31&lt;80),"B+",IF(AND(H31&gt;=70,H31&lt;75),"B",IF(AND(H31&gt;=65,H31&lt;70),"B-",IF(AND(H31&gt;=62.5,H31&lt;65),"C+",IF(AND(H31&gt;=60,H31&lt;62.5),"C",IF(AND(H31&gt;=57,H31&lt;60),"C-",IF(AND(H31&gt;=55,H31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="U31" s="16" t="str">
+      <c r="U31" s="15" t="str">
         <f t="shared" ref="U31:U34" si="11">IF(I31&gt;=85,"A",IF(AND(I31&gt;=80,I31&lt;85),"A-",IF(AND(I31&gt;=75,I31&lt;80),"B+",IF(AND(I31&gt;=70,I31&lt;75),"B",IF(AND(I31&gt;=65,I31&lt;70),"B-",IF(AND(I31&gt;=62.5,I31&lt;65),"C+",IF(AND(I31&gt;=60,I31&lt;62.5),"C",IF(AND(I31&gt;=57,I31&lt;60),"C-",IF(AND(I31&gt;=55,I31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="V31" s="16" t="str">
+      <c r="V31" s="15" t="str">
         <f t="shared" ref="V31:V34" si="12">IF(J31&gt;=85,"A",IF(AND(J31&gt;=80,J31&lt;85),"A-",IF(AND(J31&gt;=75,J31&lt;80),"B+",IF(AND(J31&gt;=70,J31&lt;75),"B",IF(AND(J31&gt;=65,J31&lt;70),"B-",IF(AND(J31&gt;=62.5,J31&lt;65),"C+",IF(AND(J31&gt;=60,J31&lt;62.5),"C",IF(AND(J31&gt;=57,J31&lt;60),"C-",IF(AND(J31&gt;=55,J31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="W31" s="16" t="str">
+      <c r="W31" s="15" t="str">
         <f t="shared" ref="W31:W34" si="13">IF(K31&gt;=85,"A",IF(AND(K31&gt;=80,K31&lt;85),"A-",IF(AND(K31&gt;=75,K31&lt;80),"B+",IF(AND(K31&gt;=70,K31&lt;75),"B",IF(AND(K31&gt;=65,K31&lt;70),"B-",IF(AND(K31&gt;=62.5,K31&lt;65),"C+",IF(AND(K31&gt;=60,K31&lt;62.5),"C",IF(AND(K31&gt;=57,K31&lt;60),"C-",IF(AND(K31&gt;=55,K31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
-      <c r="X31" s="16" t="str">
+      <c r="X31" s="15" t="str">
         <f t="shared" ref="X31:X34" si="14">IF(L31&gt;=85,"A",IF(AND(L31&gt;=80,L31&lt;85),"A-",IF(AND(L31&gt;=75,L31&lt;80),"B+",IF(AND(L31&gt;=70,L31&lt;75),"B",IF(AND(L31&gt;=65,L31&lt;70),"B-",IF(AND(L31&gt;=62.5,L31&lt;65),"C+",IF(AND(L31&gt;=60,L31&lt;62.5),"C",IF(AND(L31&gt;=57,L31&lt;60),"C-",IF(AND(L31&gt;=55,L31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
+      <c r="B32" s="3">
+        <v>29</v>
+      </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -5316,55 +5673,57 @@
       <c r="L32" s="3">
         <v>0</v>
       </c>
-      <c r="M32" s="14" t="e">
-        <f>VLOOKUP($B32,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N32" s="14" t="e">
-        <f>VLOOKUP($B32,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O32" s="14" t="e">
-        <f>VLOOKUP($B32,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P32" s="14" t="e">
-        <f>VLOOKUP($B32,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M32" s="14" t="str">
+        <f>mentee!G30</f>
+        <v>nim</v>
+      </c>
+      <c r="N32" s="14" t="str">
+        <f>mentee!D30</f>
+        <v>email</v>
+      </c>
+      <c r="O32" s="14" t="str">
+        <f>mentee!E30</f>
+        <v>univ</v>
+      </c>
+      <c r="P32" s="14" t="str">
+        <f>mentee!F30</f>
+        <v>jurusan</v>
       </c>
       <c r="Q32" s="3"/>
-      <c r="R32" s="16" t="str">
+      <c r="R32" s="15" t="str">
         <f t="shared" si="8"/>
         <v>E</v>
       </c>
-      <c r="S32" s="16" t="str">
+      <c r="S32" s="15" t="str">
         <f t="shared" si="9"/>
         <v>E</v>
       </c>
-      <c r="T32" s="16" t="str">
+      <c r="T32" s="15" t="str">
         <f t="shared" si="10"/>
         <v>E</v>
       </c>
-      <c r="U32" s="16" t="str">
+      <c r="U32" s="15" t="str">
         <f t="shared" si="11"/>
         <v>E</v>
       </c>
-      <c r="V32" s="16" t="str">
+      <c r="V32" s="15" t="str">
         <f t="shared" si="12"/>
         <v>E</v>
       </c>
-      <c r="W32" s="16" t="str">
+      <c r="W32" s="15" t="str">
         <f t="shared" si="13"/>
         <v>E</v>
       </c>
-      <c r="X32" s="16" t="str">
+      <c r="X32" s="15" t="str">
         <f t="shared" si="14"/>
         <v>E</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
+      <c r="B33" s="3">
+        <v>30</v>
+      </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -5389,48 +5748,48 @@
       <c r="L33" s="3">
         <v>0</v>
       </c>
-      <c r="M33" s="14" t="e">
-        <f>VLOOKUP($B33,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N33" s="14" t="e">
-        <f>VLOOKUP($B33,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O33" s="14" t="e">
-        <f>VLOOKUP($B33,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P33" s="14" t="e">
-        <f>VLOOKUP($B33,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M33" s="14" t="str">
+        <f>mentee!G31</f>
+        <v>nim</v>
+      </c>
+      <c r="N33" s="14" t="str">
+        <f>mentee!D31</f>
+        <v>email</v>
+      </c>
+      <c r="O33" s="14" t="str">
+        <f>mentee!E31</f>
+        <v>univ</v>
+      </c>
+      <c r="P33" s="14" t="str">
+        <f>mentee!F31</f>
+        <v>jurusan</v>
       </c>
       <c r="Q33" s="3"/>
-      <c r="R33" s="16" t="str">
+      <c r="R33" s="15" t="str">
         <f t="shared" si="8"/>
         <v>E</v>
       </c>
-      <c r="S33" s="16" t="str">
+      <c r="S33" s="15" t="str">
         <f t="shared" si="9"/>
         <v>E</v>
       </c>
-      <c r="T33" s="16" t="str">
+      <c r="T33" s="15" t="str">
         <f t="shared" si="10"/>
         <v>E</v>
       </c>
-      <c r="U33" s="16" t="str">
+      <c r="U33" s="15" t="str">
         <f t="shared" si="11"/>
         <v>E</v>
       </c>
-      <c r="V33" s="16" t="str">
+      <c r="V33" s="15" t="str">
         <f t="shared" si="12"/>
         <v>E</v>
       </c>
-      <c r="W33" s="16" t="str">
+      <c r="W33" s="15" t="str">
         <f t="shared" si="13"/>
         <v>E</v>
       </c>
-      <c r="X33" s="16" t="str">
+      <c r="X33" s="15" t="str">
         <f t="shared" si="14"/>
         <v>E</v>
       </c>
@@ -5441,72 +5800,25 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="3">
-        <v>0</v>
-      </c>
-      <c r="G34" s="3">
-        <v>0</v>
-      </c>
-      <c r="H34" s="3">
-        <v>0</v>
-      </c>
-      <c r="I34" s="3">
-        <v>0</v>
-      </c>
-      <c r="J34" s="3">
-        <v>0</v>
-      </c>
-      <c r="K34" s="3">
-        <v>0</v>
-      </c>
-      <c r="L34" s="3">
-        <v>0</v>
-      </c>
-      <c r="M34" s="14" t="e">
-        <f>VLOOKUP($B34,mentee!$B$2:$G$30,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N34" s="14" t="e">
-        <f>VLOOKUP($B34,mentee!$B$2:$G$30,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O34" s="14" t="e">
-        <f>VLOOKUP($B34,mentee!$B$2:$G$30,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P34" s="14" t="e">
-        <f>VLOOKUP($B34,mentee!$B$2:$G$30,5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
       <c r="Q34" s="3"/>
-      <c r="R34" s="16" t="str">
-        <f t="shared" si="8"/>
-        <v>E</v>
-      </c>
-      <c r="S34" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>E</v>
-      </c>
-      <c r="T34" s="16" t="str">
-        <f t="shared" si="10"/>
-        <v>E</v>
-      </c>
-      <c r="U34" s="16" t="str">
-        <f t="shared" si="11"/>
-        <v>E</v>
-      </c>
-      <c r="V34" s="16" t="str">
-        <f t="shared" si="12"/>
-        <v>E</v>
-      </c>
-      <c r="W34" s="16" t="str">
-        <f t="shared" si="13"/>
-        <v>E</v>
-      </c>
-      <c r="X34" s="16" t="str">
-        <f t="shared" si="14"/>
-        <v>E</v>
-      </c>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="15"/>
+      <c r="U34" s="15"/>
+      <c r="V34" s="15"/>
+      <c r="W34" s="15"/>
+      <c r="X34" s="15"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>

</xml_diff>

<commit_message>
tambah bobot dan total
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanfabella/Documents/kampus merdeka/script/natrya-backup-kampusmerdeka/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DA9937-0B53-1247-8CD5-70FB45457137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A1E3CC-0380-9247-A47C-A2C750A3A60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="500" windowWidth="28040" windowHeight="15620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentee" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="40">
   <si>
     <t>id peserta</t>
   </si>
@@ -111,6 +111,48 @@
   <si>
     <t>huruf_7</t>
   </si>
+  <si>
+    <t>Bobot_1</t>
+  </si>
+  <si>
+    <t>Bobot_2</t>
+  </si>
+  <si>
+    <t>Bobot_3</t>
+  </si>
+  <si>
+    <t>Bobot_4</t>
+  </si>
+  <si>
+    <t>Bobot_5</t>
+  </si>
+  <si>
+    <t>Bobot_6</t>
+  </si>
+  <si>
+    <t>Bobot_7</t>
+  </si>
+  <si>
+    <t>total_1</t>
+  </si>
+  <si>
+    <t>total_2</t>
+  </si>
+  <si>
+    <t>total_3</t>
+  </si>
+  <si>
+    <t>total_4</t>
+  </si>
+  <si>
+    <t>total_5</t>
+  </si>
+  <si>
+    <t>total_6</t>
+  </si>
+  <si>
+    <t>total_7</t>
+  </si>
 </sst>
 </file>
 
@@ -180,7 +222,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -233,11 +275,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -272,6 +340,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3463,10 +3535,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:X100"/>
+  <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AF26" sqref="AF26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3479,12 +3551,35 @@
     <col min="6" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
@@ -3540,11 +3635,53 @@
       <c r="W3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL3" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3">
         <v>1</v>
@@ -3614,12 +3751,68 @@
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
-      <c r="X4" s="15" t="str">
+      <c r="X4" s="17" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y4" s="3">
+        <f>IF(R4="A",4,IF(R4="A-",3.75,IF(R4="B+",3.5,IF(R4="B",3,IF(R4="B-",2.75,IF(R4="C+",2.25,IF(R4="C",2,IF(R4="C-",1.75,IF(R4="D",1,0)))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <f t="shared" ref="Z4:AE19" si="1">IF(S4="A",4,IF(S4="A-",3.75,IF(S4="B+",3.5,IF(S4="B",3,IF(S4="B-",2.75,IF(S4="C+",2.25,IF(S4="C",2,IF(S4="C-",1.75,IF(S4="D",1,0)))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE4" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="3">
+        <f>$F$2*Y4</f>
+        <v>0</v>
+      </c>
+      <c r="AG4" s="3">
+        <f>$G$2*Z4</f>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="3">
+        <f>$H$2*AA4</f>
+        <v>0</v>
+      </c>
+      <c r="AI4" s="3">
+        <f>$I$2*AB4</f>
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="3">
+        <f>$J$2*AC4</f>
+        <v>0</v>
+      </c>
+      <c r="AK4" s="3">
+        <f>$K$2*AD4</f>
+        <v>0</v>
+      </c>
+      <c r="AL4" s="3">
+        <f>$L$2*AE4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3">
         <v>2</v>
@@ -3666,35 +3859,91 @@
       </c>
       <c r="Q5" s="3"/>
       <c r="R5" s="15" t="str">
-        <f t="shared" ref="R5:R30" si="1">IF(F5&gt;=85,"A",IF(AND(F5&gt;=80,F5&lt;85),"A-",IF(AND(F5&gt;=75,F5&lt;80),"B+",IF(AND(F5&gt;=70,F5&lt;75),"B",IF(AND(F5&gt;=65,F5&lt;70),"B-",IF(AND(F5&gt;=62.5,F5&lt;65),"C+",IF(AND(F5&gt;=60,F5&lt;62.5),"C",IF(AND(F5&gt;=57,F5&lt;60),"C-",IF(AND(F5&gt;=55,F5&lt;57),"D","E")))))))))</f>
+        <f t="shared" ref="R5:R30" si="2">IF(F5&gt;=85,"A",IF(AND(F5&gt;=80,F5&lt;85),"A-",IF(AND(F5&gt;=75,F5&lt;80),"B+",IF(AND(F5&gt;=70,F5&lt;75),"B",IF(AND(F5&gt;=65,F5&lt;70),"B-",IF(AND(F5&gt;=62.5,F5&lt;65),"C+",IF(AND(F5&gt;=60,F5&lt;62.5),"C",IF(AND(F5&gt;=57,F5&lt;60),"C-",IF(AND(F5&gt;=55,F5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
       <c r="S5" s="15" t="str">
-        <f t="shared" ref="S5:S30" si="2">IF(G5&gt;=85,"A",IF(AND(G5&gt;=80,G5&lt;85),"A-",IF(AND(G5&gt;=75,G5&lt;80),"B+",IF(AND(G5&gt;=70,G5&lt;75),"B",IF(AND(G5&gt;=65,G5&lt;70),"B-",IF(AND(G5&gt;=62.5,G5&lt;65),"C+",IF(AND(G5&gt;=60,G5&lt;62.5),"C",IF(AND(G5&gt;=57,G5&lt;60),"C-",IF(AND(G5&gt;=55,G5&lt;57),"D","E")))))))))</f>
+        <f t="shared" ref="S5:S30" si="3">IF(G5&gt;=85,"A",IF(AND(G5&gt;=80,G5&lt;85),"A-",IF(AND(G5&gt;=75,G5&lt;80),"B+",IF(AND(G5&gt;=70,G5&lt;75),"B",IF(AND(G5&gt;=65,G5&lt;70),"B-",IF(AND(G5&gt;=62.5,G5&lt;65),"C+",IF(AND(G5&gt;=60,G5&lt;62.5),"C",IF(AND(G5&gt;=57,G5&lt;60),"C-",IF(AND(G5&gt;=55,G5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
       <c r="T5" s="15" t="str">
-        <f t="shared" ref="T5:T30" si="3">IF(H5&gt;=85,"A",IF(AND(H5&gt;=80,H5&lt;85),"A-",IF(AND(H5&gt;=75,H5&lt;80),"B+",IF(AND(H5&gt;=70,H5&lt;75),"B",IF(AND(H5&gt;=65,H5&lt;70),"B-",IF(AND(H5&gt;=62.5,H5&lt;65),"C+",IF(AND(H5&gt;=60,H5&lt;62.5),"C",IF(AND(H5&gt;=57,H5&lt;60),"C-",IF(AND(H5&gt;=55,H5&lt;57),"D","E")))))))))</f>
+        <f t="shared" ref="T5:T30" si="4">IF(H5&gt;=85,"A",IF(AND(H5&gt;=80,H5&lt;85),"A-",IF(AND(H5&gt;=75,H5&lt;80),"B+",IF(AND(H5&gt;=70,H5&lt;75),"B",IF(AND(H5&gt;=65,H5&lt;70),"B-",IF(AND(H5&gt;=62.5,H5&lt;65),"C+",IF(AND(H5&gt;=60,H5&lt;62.5),"C",IF(AND(H5&gt;=57,H5&lt;60),"C-",IF(AND(H5&gt;=55,H5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
       <c r="U5" s="15" t="str">
-        <f t="shared" ref="U5:U30" si="4">IF(I5&gt;=85,"A",IF(AND(I5&gt;=80,I5&lt;85),"A-",IF(AND(I5&gt;=75,I5&lt;80),"B+",IF(AND(I5&gt;=70,I5&lt;75),"B",IF(AND(I5&gt;=65,I5&lt;70),"B-",IF(AND(I5&gt;=62.5,I5&lt;65),"C+",IF(AND(I5&gt;=60,I5&lt;62.5),"C",IF(AND(I5&gt;=57,I5&lt;60),"C-",IF(AND(I5&gt;=55,I5&lt;57),"D","E")))))))))</f>
+        <f t="shared" ref="U5:U30" si="5">IF(I5&gt;=85,"A",IF(AND(I5&gt;=80,I5&lt;85),"A-",IF(AND(I5&gt;=75,I5&lt;80),"B+",IF(AND(I5&gt;=70,I5&lt;75),"B",IF(AND(I5&gt;=65,I5&lt;70),"B-",IF(AND(I5&gt;=62.5,I5&lt;65),"C+",IF(AND(I5&gt;=60,I5&lt;62.5),"C",IF(AND(I5&gt;=57,I5&lt;60),"C-",IF(AND(I5&gt;=55,I5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
       <c r="V5" s="15" t="str">
-        <f t="shared" ref="V5:V30" si="5">IF(J5&gt;=85,"A",IF(AND(J5&gt;=80,J5&lt;85),"A-",IF(AND(J5&gt;=75,J5&lt;80),"B+",IF(AND(J5&gt;=70,J5&lt;75),"B",IF(AND(J5&gt;=65,J5&lt;70),"B-",IF(AND(J5&gt;=62.5,J5&lt;65),"C+",IF(AND(J5&gt;=60,J5&lt;62.5),"C",IF(AND(J5&gt;=57,J5&lt;60),"C-",IF(AND(J5&gt;=55,J5&lt;57),"D","E")))))))))</f>
+        <f t="shared" ref="V5:V30" si="6">IF(J5&gt;=85,"A",IF(AND(J5&gt;=80,J5&lt;85),"A-",IF(AND(J5&gt;=75,J5&lt;80),"B+",IF(AND(J5&gt;=70,J5&lt;75),"B",IF(AND(J5&gt;=65,J5&lt;70),"B-",IF(AND(J5&gt;=62.5,J5&lt;65),"C+",IF(AND(J5&gt;=60,J5&lt;62.5),"C",IF(AND(J5&gt;=57,J5&lt;60),"C-",IF(AND(J5&gt;=55,J5&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
       <c r="W5" s="15" t="str">
-        <f t="shared" ref="W5:W30" si="6">IF(K5&gt;=85,"A",IF(AND(K5&gt;=80,K5&lt;85),"A-",IF(AND(K5&gt;=75,K5&lt;80),"B+",IF(AND(K5&gt;=70,K5&lt;75),"B",IF(AND(K5&gt;=65,K5&lt;70),"B-",IF(AND(K5&gt;=62.5,K5&lt;65),"C+",IF(AND(K5&gt;=60,K5&lt;62.5),"C",IF(AND(K5&gt;=57,K5&lt;60),"C-",IF(AND(K5&gt;=55,K5&lt;57),"D","E")))))))))</f>
-        <v>E</v>
-      </c>
-      <c r="X5" s="15" t="str">
-        <f t="shared" ref="X5:X30" si="7">IF(L5&gt;=85,"A",IF(AND(L5&gt;=80,L5&lt;85),"A-",IF(AND(L5&gt;=75,L5&lt;80),"B+",IF(AND(L5&gt;=70,L5&lt;75),"B",IF(AND(L5&gt;=65,L5&lt;70),"B-",IF(AND(L5&gt;=62.5,L5&lt;65),"C+",IF(AND(L5&gt;=60,L5&lt;62.5),"C",IF(AND(L5&gt;=57,L5&lt;60),"C-",IF(AND(L5&gt;=55,L5&lt;57),"D","E")))))))))</f>
-        <v>E</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+        <f t="shared" ref="W5:W30" si="7">IF(K5&gt;=85,"A",IF(AND(K5&gt;=80,K5&lt;85),"A-",IF(AND(K5&gt;=75,K5&lt;80),"B+",IF(AND(K5&gt;=70,K5&lt;75),"B",IF(AND(K5&gt;=65,K5&lt;70),"B-",IF(AND(K5&gt;=62.5,K5&lt;65),"C+",IF(AND(K5&gt;=60,K5&lt;62.5),"C",IF(AND(K5&gt;=57,K5&lt;60),"C-",IF(AND(K5&gt;=55,K5&lt;57),"D","E")))))))))</f>
+        <v>E</v>
+      </c>
+      <c r="X5" s="17" t="str">
+        <f t="shared" ref="X5:X30" si="8">IF(L5&gt;=85,"A",IF(AND(L5&gt;=80,L5&lt;85),"A-",IF(AND(L5&gt;=75,L5&lt;80),"B+",IF(AND(L5&gt;=70,L5&lt;75),"B",IF(AND(L5&gt;=65,L5&lt;70),"B-",IF(AND(L5&gt;=62.5,L5&lt;65),"C+",IF(AND(L5&gt;=60,L5&lt;62.5),"C",IF(AND(L5&gt;=57,L5&lt;60),"C-",IF(AND(L5&gt;=55,L5&lt;57),"D","E")))))))))</f>
+        <v>E</v>
+      </c>
+      <c r="Y5" s="3">
+        <f t="shared" ref="Y5:Y33" si="9">IF(R5="A",4,IF(R5="A-",3.75,IF(R5="B+",3.5,IF(R5="B",3,IF(R5="B-",2.75,IF(R5="C+",2.25,IF(R5="C",2,IF(R5="C-",1.75,IF(R5="D",1,0)))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="3">
+        <f t="shared" ref="AF5:AF33" si="10">$F$2*Y5</f>
+        <v>0</v>
+      </c>
+      <c r="AG5" s="3">
+        <f t="shared" ref="AG5:AG33" si="11">$G$2*Z5</f>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="3">
+        <f t="shared" ref="AH5:AH33" si="12">$H$2*AA5</f>
+        <v>0</v>
+      </c>
+      <c r="AI5" s="3">
+        <f t="shared" ref="AI5:AI33" si="13">$I$2*AB5</f>
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="3">
+        <f t="shared" ref="AJ5:AJ33" si="14">$J$2*AC5</f>
+        <v>0</v>
+      </c>
+      <c r="AK5" s="3">
+        <f t="shared" ref="AK5:AK33" si="15">$K$2*AD5</f>
+        <v>0</v>
+      </c>
+      <c r="AL5" s="3">
+        <f t="shared" ref="AL5:AL33" si="16">$L$2*AE5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <v>3</v>
@@ -3741,35 +3990,91 @@
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S6" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T6" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U6" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V6" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W6" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X6" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X6" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y6" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK6" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL6" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3">
         <v>4</v>
@@ -3816,35 +4121,91 @@
       </c>
       <c r="Q7" s="3"/>
       <c r="R7" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S7" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T7" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U7" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V7" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W7" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X7" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X7" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y7" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH7" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI7" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK7" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL7" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3">
         <v>5</v>
@@ -3891,35 +4252,91 @@
       </c>
       <c r="Q8" s="3"/>
       <c r="R8" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S8" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T8" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U8" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V8" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W8" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X8" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X8" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y8" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH8" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK8" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL8" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3">
         <v>6</v>
@@ -3966,35 +4383,91 @@
       </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S9" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T9" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U9" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V9" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W9" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X9" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X9" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y9" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF9" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG9" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH9" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI9" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK9" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL9" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3">
         <v>7</v>
@@ -4041,35 +4514,91 @@
       </c>
       <c r="Q10" s="3"/>
       <c r="R10" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S10" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T10" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U10" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V10" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W10" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X10" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X10" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y10" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF10" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG10" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH10" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI10" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK10" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL10" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3">
         <v>8</v>
@@ -4116,35 +4645,91 @@
       </c>
       <c r="Q11" s="3"/>
       <c r="R11" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S11" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T11" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U11" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V11" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W11" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X11" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X11" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y11" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG11" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH11" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI11" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK11" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL11" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3">
         <v>9</v>
@@ -4191,35 +4776,91 @@
       </c>
       <c r="Q12" s="3"/>
       <c r="R12" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S12" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T12" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U12" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V12" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W12" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X12" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X12" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y12" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF12" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG12" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH12" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI12" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK12" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL12" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3">
         <v>10</v>
@@ -4266,35 +4907,91 @@
       </c>
       <c r="Q13" s="3"/>
       <c r="R13" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S13" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T13" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U13" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V13" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W13" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X13" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X13" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y13" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF13" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG13" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH13" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI13" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK13" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL13" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
         <v>11</v>
@@ -4341,35 +5038,91 @@
       </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S14" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T14" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U14" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V14" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W14" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X14" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X14" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y14" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF14" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG14" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH14" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI14" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK14" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL14" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3">
         <v>12</v>
@@ -4416,35 +5169,91 @@
       </c>
       <c r="Q15" s="3"/>
       <c r="R15" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S15" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T15" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U15" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V15" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W15" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X15" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X15" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y15" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF15" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG15" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH15" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI15" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK15" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL15" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3">
         <v>13</v>
@@ -4491,35 +5300,91 @@
       </c>
       <c r="Q16" s="3"/>
       <c r="R16" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S16" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T16" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U16" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V16" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W16" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X16" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X16" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y16" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF16" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG16" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH16" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI16" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK16" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL16" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3">
         <v>14</v>
@@ -4566,35 +5431,91 @@
       </c>
       <c r="Q17" s="3"/>
       <c r="R17" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S17" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T17" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U17" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V17" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W17" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X17" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X17" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y17" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF17" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG17" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH17" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI17" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK17" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL17" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3">
         <v>15</v>
@@ -4641,35 +5562,91 @@
       </c>
       <c r="Q18" s="3"/>
       <c r="R18" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S18" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T18" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U18" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V18" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W18" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X18" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X18" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y18" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF18" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG18" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH18" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI18" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK18" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL18" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3">
         <v>16</v>
@@ -4716,35 +5693,91 @@
       </c>
       <c r="Q19" s="3"/>
       <c r="R19" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S19" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T19" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U19" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V19" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W19" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X19" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X19" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y19" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF19" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG19" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH19" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI19" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK19" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL19" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3">
         <v>17</v>
@@ -4791,35 +5824,91 @@
       </c>
       <c r="Q20" s="3"/>
       <c r="R20" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S20" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T20" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U20" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V20" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W20" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X20" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X20" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y20" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z20" s="3">
+        <f t="shared" ref="Z20:Z33" si="17">IF(S20="A",4,IF(S20="A-",3.75,IF(S20="B+",3.5,IF(S20="B",3,IF(S20="B-",2.75,IF(S20="C+",2.25,IF(S20="C",2,IF(S20="C-",1.75,IF(S20="D",1,0)))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="AA20" s="3">
+        <f t="shared" ref="AA20:AA33" si="18">IF(T20="A",4,IF(T20="A-",3.75,IF(T20="B+",3.5,IF(T20="B",3,IF(T20="B-",2.75,IF(T20="C+",2.25,IF(T20="C",2,IF(T20="C-",1.75,IF(T20="D",1,0)))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="AB20" s="3">
+        <f t="shared" ref="AB20:AB33" si="19">IF(U20="A",4,IF(U20="A-",3.75,IF(U20="B+",3.5,IF(U20="B",3,IF(U20="B-",2.75,IF(U20="C+",2.25,IF(U20="C",2,IF(U20="C-",1.75,IF(U20="D",1,0)))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="AC20" s="3">
+        <f t="shared" ref="AC20:AC33" si="20">IF(V20="A",4,IF(V20="A-",3.75,IF(V20="B+",3.5,IF(V20="B",3,IF(V20="B-",2.75,IF(V20="C+",2.25,IF(V20="C",2,IF(V20="C-",1.75,IF(V20="D",1,0)))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="AD20" s="3">
+        <f t="shared" ref="AD20:AD33" si="21">IF(W20="A",4,IF(W20="A-",3.75,IF(W20="B+",3.5,IF(W20="B",3,IF(W20="B-",2.75,IF(W20="C+",2.25,IF(W20="C",2,IF(W20="C-",1.75,IF(W20="D",1,0)))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="AE20" s="3">
+        <f t="shared" ref="AE20:AE33" si="22">IF(X20="A",4,IF(X20="A-",3.75,IF(X20="B+",3.5,IF(X20="B",3,IF(X20="B-",2.75,IF(X20="C+",2.25,IF(X20="C",2,IF(X20="C-",1.75,IF(X20="D",1,0)))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="AF20" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG20" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH20" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI20" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK20" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL20" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3">
         <v>18</v>
@@ -4866,35 +5955,91 @@
       </c>
       <c r="Q21" s="3"/>
       <c r="R21" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S21" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T21" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U21" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V21" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W21" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X21" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X21" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y21" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB21" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC21" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD21" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE21" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF21" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG21" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH21" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI21" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK21" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL21" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3">
         <v>19</v>
@@ -4941,35 +6086,91 @@
       </c>
       <c r="Q22" s="3"/>
       <c r="R22" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S22" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T22" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U22" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V22" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W22" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X22" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X22" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y22" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD22" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE22" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF22" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG22" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH22" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI22" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK22" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL22" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3">
         <v>20</v>
@@ -5016,35 +6217,91 @@
       </c>
       <c r="Q23" s="3"/>
       <c r="R23" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S23" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T23" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U23" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V23" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W23" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X23" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X23" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y23" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC23" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD23" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE23" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF23" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG23" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH23" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI23" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK23" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL23" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3">
         <v>21</v>
@@ -5091,35 +6348,91 @@
       </c>
       <c r="Q24" s="3"/>
       <c r="R24" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S24" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T24" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U24" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V24" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W24" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X24" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X24" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y24" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC24" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE24" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG24" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH24" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI24" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK24" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL24" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3">
         <v>22</v>
@@ -5166,35 +6479,91 @@
       </c>
       <c r="Q25" s="3"/>
       <c r="R25" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S25" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T25" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U25" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V25" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W25" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X25" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X25" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y25" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z25" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA25" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB25" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC25" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD25" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE25" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF25" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG25" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH25" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI25" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK25" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL25" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3">
         <v>23</v>
@@ -5241,35 +6610,91 @@
       </c>
       <c r="Q26" s="3"/>
       <c r="R26" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S26" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T26" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U26" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V26" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W26" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X26" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X26" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y26" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z26" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA26" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB26" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC26" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD26" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE26" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF26" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG26" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH26" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI26" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK26" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL26" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3">
         <v>24</v>
@@ -5316,35 +6741,91 @@
       </c>
       <c r="Q27" s="3"/>
       <c r="R27" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S27" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T27" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U27" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V27" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W27" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X27" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X27" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y27" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z27" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA27" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB27" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC27" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD27" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE27" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF27" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG27" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH27" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI27" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK27" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL27" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3">
         <v>25</v>
@@ -5391,35 +6872,91 @@
       </c>
       <c r="Q28" s="3"/>
       <c r="R28" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S28" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T28" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U28" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V28" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W28" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X28" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X28" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y28" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z28" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA28" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB28" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC28" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD28" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE28" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF28" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG28" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH28" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI28" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK28" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL28" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3">
         <v>26</v>
@@ -5466,35 +7003,91 @@
       </c>
       <c r="Q29" s="3"/>
       <c r="R29" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S29" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T29" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U29" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V29" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W29" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X29" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X29" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y29" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB29" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC29" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD29" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE29" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF29" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG29" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH29" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI29" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ29" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK29" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL29" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3">
         <v>27</v>
@@ -5541,35 +7134,91 @@
       </c>
       <c r="Q30" s="3"/>
       <c r="R30" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
       <c r="S30" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E</v>
       </c>
       <c r="T30" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="U30" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="V30" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="W30" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
-      </c>
-      <c r="X30" s="15" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X30" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="Y30" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA30" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB30" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC30" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD30" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE30" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF30" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG30" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH30" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI30" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ30" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK30" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL30" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3">
         <v>28</v>
@@ -5616,35 +7265,91 @@
       </c>
       <c r="Q31" s="3"/>
       <c r="R31" s="15" t="str">
-        <f t="shared" ref="R31:R34" si="8">IF(F31&gt;=85,"A",IF(AND(F31&gt;=80,F31&lt;85),"A-",IF(AND(F31&gt;=75,F31&lt;80),"B+",IF(AND(F31&gt;=70,F31&lt;75),"B",IF(AND(F31&gt;=65,F31&lt;70),"B-",IF(AND(F31&gt;=62.5,F31&lt;65),"C+",IF(AND(F31&gt;=60,F31&lt;62.5),"C",IF(AND(F31&gt;=57,F31&lt;60),"C-",IF(AND(F31&gt;=55,F31&lt;57),"D","E")))))))))</f>
+        <f t="shared" ref="R31:R33" si="23">IF(F31&gt;=85,"A",IF(AND(F31&gt;=80,F31&lt;85),"A-",IF(AND(F31&gt;=75,F31&lt;80),"B+",IF(AND(F31&gt;=70,F31&lt;75),"B",IF(AND(F31&gt;=65,F31&lt;70),"B-",IF(AND(F31&gt;=62.5,F31&lt;65),"C+",IF(AND(F31&gt;=60,F31&lt;62.5),"C",IF(AND(F31&gt;=57,F31&lt;60),"C-",IF(AND(F31&gt;=55,F31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
       <c r="S31" s="15" t="str">
-        <f t="shared" ref="S31:S34" si="9">IF(G31&gt;=85,"A",IF(AND(G31&gt;=80,G31&lt;85),"A-",IF(AND(G31&gt;=75,G31&lt;80),"B+",IF(AND(G31&gt;=70,G31&lt;75),"B",IF(AND(G31&gt;=65,G31&lt;70),"B-",IF(AND(G31&gt;=62.5,G31&lt;65),"C+",IF(AND(G31&gt;=60,G31&lt;62.5),"C",IF(AND(G31&gt;=57,G31&lt;60),"C-",IF(AND(G31&gt;=55,G31&lt;57),"D","E")))))))))</f>
+        <f t="shared" ref="S31:S33" si="24">IF(G31&gt;=85,"A",IF(AND(G31&gt;=80,G31&lt;85),"A-",IF(AND(G31&gt;=75,G31&lt;80),"B+",IF(AND(G31&gt;=70,G31&lt;75),"B",IF(AND(G31&gt;=65,G31&lt;70),"B-",IF(AND(G31&gt;=62.5,G31&lt;65),"C+",IF(AND(G31&gt;=60,G31&lt;62.5),"C",IF(AND(G31&gt;=57,G31&lt;60),"C-",IF(AND(G31&gt;=55,G31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
       <c r="T31" s="15" t="str">
-        <f t="shared" ref="T31:T34" si="10">IF(H31&gt;=85,"A",IF(AND(H31&gt;=80,H31&lt;85),"A-",IF(AND(H31&gt;=75,H31&lt;80),"B+",IF(AND(H31&gt;=70,H31&lt;75),"B",IF(AND(H31&gt;=65,H31&lt;70),"B-",IF(AND(H31&gt;=62.5,H31&lt;65),"C+",IF(AND(H31&gt;=60,H31&lt;62.5),"C",IF(AND(H31&gt;=57,H31&lt;60),"C-",IF(AND(H31&gt;=55,H31&lt;57),"D","E")))))))))</f>
+        <f t="shared" ref="T31:T33" si="25">IF(H31&gt;=85,"A",IF(AND(H31&gt;=80,H31&lt;85),"A-",IF(AND(H31&gt;=75,H31&lt;80),"B+",IF(AND(H31&gt;=70,H31&lt;75),"B",IF(AND(H31&gt;=65,H31&lt;70),"B-",IF(AND(H31&gt;=62.5,H31&lt;65),"C+",IF(AND(H31&gt;=60,H31&lt;62.5),"C",IF(AND(H31&gt;=57,H31&lt;60),"C-",IF(AND(H31&gt;=55,H31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
       <c r="U31" s="15" t="str">
-        <f t="shared" ref="U31:U34" si="11">IF(I31&gt;=85,"A",IF(AND(I31&gt;=80,I31&lt;85),"A-",IF(AND(I31&gt;=75,I31&lt;80),"B+",IF(AND(I31&gt;=70,I31&lt;75),"B",IF(AND(I31&gt;=65,I31&lt;70),"B-",IF(AND(I31&gt;=62.5,I31&lt;65),"C+",IF(AND(I31&gt;=60,I31&lt;62.5),"C",IF(AND(I31&gt;=57,I31&lt;60),"C-",IF(AND(I31&gt;=55,I31&lt;57),"D","E")))))))))</f>
+        <f t="shared" ref="U31:U33" si="26">IF(I31&gt;=85,"A",IF(AND(I31&gt;=80,I31&lt;85),"A-",IF(AND(I31&gt;=75,I31&lt;80),"B+",IF(AND(I31&gt;=70,I31&lt;75),"B",IF(AND(I31&gt;=65,I31&lt;70),"B-",IF(AND(I31&gt;=62.5,I31&lt;65),"C+",IF(AND(I31&gt;=60,I31&lt;62.5),"C",IF(AND(I31&gt;=57,I31&lt;60),"C-",IF(AND(I31&gt;=55,I31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
       <c r="V31" s="15" t="str">
-        <f t="shared" ref="V31:V34" si="12">IF(J31&gt;=85,"A",IF(AND(J31&gt;=80,J31&lt;85),"A-",IF(AND(J31&gt;=75,J31&lt;80),"B+",IF(AND(J31&gt;=70,J31&lt;75),"B",IF(AND(J31&gt;=65,J31&lt;70),"B-",IF(AND(J31&gt;=62.5,J31&lt;65),"C+",IF(AND(J31&gt;=60,J31&lt;62.5),"C",IF(AND(J31&gt;=57,J31&lt;60),"C-",IF(AND(J31&gt;=55,J31&lt;57),"D","E")))))))))</f>
+        <f t="shared" ref="V31:V33" si="27">IF(J31&gt;=85,"A",IF(AND(J31&gt;=80,J31&lt;85),"A-",IF(AND(J31&gt;=75,J31&lt;80),"B+",IF(AND(J31&gt;=70,J31&lt;75),"B",IF(AND(J31&gt;=65,J31&lt;70),"B-",IF(AND(J31&gt;=62.5,J31&lt;65),"C+",IF(AND(J31&gt;=60,J31&lt;62.5),"C",IF(AND(J31&gt;=57,J31&lt;60),"C-",IF(AND(J31&gt;=55,J31&lt;57),"D","E")))))))))</f>
         <v>E</v>
       </c>
       <c r="W31" s="15" t="str">
-        <f t="shared" ref="W31:W34" si="13">IF(K31&gt;=85,"A",IF(AND(K31&gt;=80,K31&lt;85),"A-",IF(AND(K31&gt;=75,K31&lt;80),"B+",IF(AND(K31&gt;=70,K31&lt;75),"B",IF(AND(K31&gt;=65,K31&lt;70),"B-",IF(AND(K31&gt;=62.5,K31&lt;65),"C+",IF(AND(K31&gt;=60,K31&lt;62.5),"C",IF(AND(K31&gt;=57,K31&lt;60),"C-",IF(AND(K31&gt;=55,K31&lt;57),"D","E")))))))))</f>
-        <v>E</v>
-      </c>
-      <c r="X31" s="15" t="str">
-        <f t="shared" ref="X31:X34" si="14">IF(L31&gt;=85,"A",IF(AND(L31&gt;=80,L31&lt;85),"A-",IF(AND(L31&gt;=75,L31&lt;80),"B+",IF(AND(L31&gt;=70,L31&lt;75),"B",IF(AND(L31&gt;=65,L31&lt;70),"B-",IF(AND(L31&gt;=62.5,L31&lt;65),"C+",IF(AND(L31&gt;=60,L31&lt;62.5),"C",IF(AND(L31&gt;=57,L31&lt;60),"C-",IF(AND(L31&gt;=55,L31&lt;57),"D","E")))))))))</f>
-        <v>E</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+        <f t="shared" ref="W31:W33" si="28">IF(K31&gt;=85,"A",IF(AND(K31&gt;=80,K31&lt;85),"A-",IF(AND(K31&gt;=75,K31&lt;80),"B+",IF(AND(K31&gt;=70,K31&lt;75),"B",IF(AND(K31&gt;=65,K31&lt;70),"B-",IF(AND(K31&gt;=62.5,K31&lt;65),"C+",IF(AND(K31&gt;=60,K31&lt;62.5),"C",IF(AND(K31&gt;=57,K31&lt;60),"C-",IF(AND(K31&gt;=55,K31&lt;57),"D","E")))))))))</f>
+        <v>E</v>
+      </c>
+      <c r="X31" s="17" t="str">
+        <f t="shared" ref="X31:X33" si="29">IF(L31&gt;=85,"A",IF(AND(L31&gt;=80,L31&lt;85),"A-",IF(AND(L31&gt;=75,L31&lt;80),"B+",IF(AND(L31&gt;=70,L31&lt;75),"B",IF(AND(L31&gt;=65,L31&lt;70),"B-",IF(AND(L31&gt;=62.5,L31&lt;65),"C+",IF(AND(L31&gt;=60,L31&lt;62.5),"C",IF(AND(L31&gt;=57,L31&lt;60),"C-",IF(AND(L31&gt;=55,L31&lt;57),"D","E")))))))))</f>
+        <v>E</v>
+      </c>
+      <c r="Y31" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA31" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC31" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD31" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE31" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF31" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG31" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH31" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI31" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AJ31" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AK31" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL31" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3">
         <v>29</v>
@@ -5691,35 +7396,91 @@
       </c>
       <c r="Q32" s="3"/>
       <c r="R32" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="23"/>
         <v>E</v>
       </c>
       <c r="S32" s="15" t="str">
+        <f t="shared" si="24"/>
+        <v>E</v>
+      </c>
+      <c r="T32" s="15" t="str">
+        <f t="shared" si="25"/>
+        <v>E</v>
+      </c>
+      <c r="U32" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>E</v>
+      </c>
+      <c r="V32" s="15" t="str">
+        <f t="shared" si="27"/>
+        <v>E</v>
+      </c>
+      <c r="W32" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>E</v>
+      </c>
+      <c r="X32" s="17" t="str">
+        <f t="shared" si="29"/>
+        <v>E</v>
+      </c>
+      <c r="Y32" s="3">
         <f t="shared" si="9"/>
-        <v>E</v>
-      </c>
-      <c r="T32" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA32" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB32" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC32" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD32" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE32" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF32" s="3">
         <f t="shared" si="10"/>
-        <v>E</v>
-      </c>
-      <c r="U32" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="3">
         <f t="shared" si="11"/>
-        <v>E</v>
-      </c>
-      <c r="V32" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="3">
         <f t="shared" si="12"/>
-        <v>E</v>
-      </c>
-      <c r="W32" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="3">
         <f t="shared" si="13"/>
-        <v>E</v>
-      </c>
-      <c r="X32" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ32" s="3">
         <f t="shared" si="14"/>
-        <v>E</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="AK32" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL32" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3">
         <v>30</v>
@@ -5766,35 +7527,91 @@
       </c>
       <c r="Q33" s="3"/>
       <c r="R33" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="23"/>
         <v>E</v>
       </c>
       <c r="S33" s="15" t="str">
+        <f t="shared" si="24"/>
+        <v>E</v>
+      </c>
+      <c r="T33" s="15" t="str">
+        <f t="shared" si="25"/>
+        <v>E</v>
+      </c>
+      <c r="U33" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>E</v>
+      </c>
+      <c r="V33" s="15" t="str">
+        <f t="shared" si="27"/>
+        <v>E</v>
+      </c>
+      <c r="W33" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>E</v>
+      </c>
+      <c r="X33" s="17" t="str">
+        <f t="shared" si="29"/>
+        <v>E</v>
+      </c>
+      <c r="Y33" s="3">
         <f t="shared" si="9"/>
-        <v>E</v>
-      </c>
-      <c r="T33" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA33" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB33" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AC33" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AD33" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE33" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF33" s="3">
         <f t="shared" si="10"/>
-        <v>E</v>
-      </c>
-      <c r="U33" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="3">
         <f t="shared" si="11"/>
-        <v>E</v>
-      </c>
-      <c r="V33" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="3">
         <f t="shared" si="12"/>
-        <v>E</v>
-      </c>
-      <c r="W33" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AI33" s="3">
         <f t="shared" si="13"/>
-        <v>E</v>
-      </c>
-      <c r="X33" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ33" s="3">
         <f t="shared" si="14"/>
-        <v>E</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL33" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5820,7 +7637,7 @@
       <c r="W34" s="15"/>
       <c r="X34" s="15"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5846,7 +7663,7 @@
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5872,7 +7689,7 @@
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5898,7 +7715,7 @@
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5924,7 +7741,7 @@
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -5950,7 +7767,7 @@
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -5976,7 +7793,7 @@
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -6002,7 +7819,7 @@
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -6028,7 +7845,7 @@
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -6054,7 +7871,7 @@
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -6080,7 +7897,7 @@
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -6106,7 +7923,7 @@
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -6132,7 +7949,7 @@
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -6158,7 +7975,7 @@
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>

</xml_diff>